<commit_message>
Included plots, Spreadsheet with sensor information and Experiment with SNR vs Accuracy for LSM-303c
</commit_message>
<xml_diff>
--- a/simulation-of-distance-with-racing-track/SNR-SENSORS.xlsx
+++ b/simulation-of-distance-with-racing-track/SNR-SENSORS.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26600" windowHeight="21400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26600" windowHeight="21400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 2 - Accuracy Racing Track" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,26 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>MPU-9250</t>
   </si>
   <si>
-    <t>MMC3416</t>
-  </si>
-  <si>
     <t>AK0991</t>
   </si>
   <si>
-    <t>Daniel's Phone</t>
-  </si>
-  <si>
     <t>Arthur's Phone</t>
   </si>
   <si>
-    <t>FXOS8700</t>
-  </si>
-  <si>
     <t>Distance Simulation in terms of SNR</t>
   </si>
   <si>
@@ -57,34 +49,28 @@
     <t>180mm</t>
   </si>
   <si>
-    <t>Algorithm #1 (Polling)</t>
-  </si>
-  <si>
-    <t>Experiment #2 - Accuracy</t>
-  </si>
-  <si>
-    <t>BASELINE</t>
-  </si>
-  <si>
-    <t>Threshold 1 / 2</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>LSM-303C</t>
+  </si>
+  <si>
+    <t>100mm</t>
+  </si>
+  <si>
+    <t>120mm</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>accuracy (/20)</t>
+  </si>
+  <si>
+    <t>interrupt</t>
+  </si>
+  <si>
+    <t>Threshold</t>
   </si>
 </sst>
 </file>
@@ -116,18 +102,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,7 +119,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,17 +157,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -206,6 +209,19 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -224,48 +240,24 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E12:J16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="E12:J16"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Threshold 1 / 2"/>
-    <tableColumn id="2" name="2" dataDxfId="6"/>
-    <tableColumn id="3" name="4" dataDxfId="5"/>
-    <tableColumn id="4" name="6" dataDxfId="4"/>
-    <tableColumn id="5" name="8" dataDxfId="3"/>
-    <tableColumn id="6" name="10" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N16"/>
+  <dimension ref="B2:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M11:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,7 +598,7 @@
     <col min="12" max="12" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:15">
       <c r="D2">
         <v>30</v>
       </c>
@@ -622,8 +614,11 @@
       <c r="H2">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="2:14">
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -647,55 +642,33 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f>(67.8-60.8)/(63.5-61.4)</f>
-        <v>3.3333333333333313</v>
-      </c>
-      <c r="E4">
-        <f>(64.7-59.5)/(62.9-60.9)</f>
-        <v>2.6000000000000014</v>
-      </c>
-      <c r="F4">
-        <f>(63-59.5)/(62.1-60.8)</f>
-        <v>2.6923076923076836</v>
-      </c>
-      <c r="G4">
-        <f>(62.4-59.8)</f>
-        <v>2.6000000000000014</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="N4">
         <f>(82.7-69.3)/(79.5-73.4)</f>
         <v>2.1967213114754127</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
+      <c r="O4">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f>(85.5-72.9)/(78.4-72.8)</f>
@@ -717,153 +690,411 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N5">
         <f>(77.5-69)/(76.5-70.9)</f>
         <v>1.5178571428571443</v>
       </c>
-    </row>
-    <row r="6" spans="2:14">
+      <c r="O5">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
       <c r="C6" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <f>(67.8-60.8)/(63.5-61.4)</f>
+        <v>3.3333333333333313</v>
+      </c>
+      <c r="E6">
+        <f>(64.7-59.5)/(62.7-60.9)</f>
+        <v>2.8888888888888835</v>
+      </c>
+      <c r="F6">
+        <f>(63-59.5)/(62.1-60.8)</f>
+        <v>2.6923076923076836</v>
+      </c>
+      <c r="G6">
+        <v>1.4568000000000001</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="N6">
         <f>(74.4-67.8)/(74.1-68.8)</f>
         <v>1.2452830188679267</v>
       </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="O6">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="M7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="1">
-        <v>20</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="O7">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="L10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="M11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>3.32897</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12">
+        <f>(38.7-29.8)/(37.3-34.3)</f>
+        <v>2.9666666666666672</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="M13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <v>2.6922999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="M14" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="1">
-        <v>2.1960000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="E13">
+      <c r="N14">
+        <f>(37.7-34.6)/(37.6-35.5)</f>
+        <v>1.4761904761904758</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="M15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15">
         <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>68</v>
-      </c>
-      <c r="G13" s="1">
-        <v>52</v>
-      </c>
-      <c r="H13" s="1">
-        <v>49</v>
-      </c>
-      <c r="I13" s="1">
-        <v>41</v>
-      </c>
-      <c r="J13" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14">
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14" s="1">
-        <v>26</v>
-      </c>
-      <c r="G14" s="1">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2">
-        <v>18</v>
-      </c>
-      <c r="I14" s="2">
-        <v>18</v>
-      </c>
-      <c r="J14" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="1">
-        <v>9</v>
-      </c>
-      <c r="H15" s="1">
-        <v>9</v>
-      </c>
-      <c r="I15" s="1">
-        <v>11</v>
-      </c>
-      <c r="J15" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="1">
-        <v>4</v>
-      </c>
-      <c r="H16" s="1">
-        <v>6</v>
-      </c>
-      <c r="I16" s="1">
-        <v>7</v>
-      </c>
-      <c r="J16" s="1">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <v>36</v>
+      </c>
+      <c r="K3">
+        <v>47</v>
+      </c>
+      <c r="L3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>3.5</v>
+      </c>
+      <c r="I4">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>37</v>
+      </c>
+      <c r="L4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>72</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>27</v>
+      </c>
+      <c r="L5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="H6">
+        <v>4.5</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>21</v>
+      </c>
+      <c r="K6">
+        <v>26</v>
+      </c>
+      <c r="L6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>21</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>23</v>
+      </c>
+      <c r="L7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="H8">
+        <v>5.5</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>22</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>19</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="H10">
+        <v>6.5</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>22</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
+      </c>
+      <c r="K11">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="H12">
+        <v>7.5</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="H14">
+        <v>8.5</v>
+      </c>
+      <c r="I14">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="K15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11">
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>20</v>
+      </c>
+      <c r="J17">
+        <v>20</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11">
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11">
+      <c r="H22">
+        <v>15</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>